<commit_message>
Added navigating to download reports, downloading reports, and navigating to upload reports
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amedeloitte-my.sharepoint.com/personal/dsembiante_deloitte_com/Documents/UiPathAcademyArcitect/GenerateYearlyReport-Performer/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B631F639-37E8-4C90-A3AA-A4F68B30FEBD}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1287EAD9-2E76-4107-9C28-40847435431C}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -186,6 +186,60 @@
   </si>
   <si>
     <t>https://acme-test.uipath.com/</t>
+  </si>
+  <si>
+    <t>System1_ReportsPath</t>
+  </si>
+  <si>
+    <t>reports/</t>
+  </si>
+  <si>
+    <t>System1_ReportsDownload</t>
+  </si>
+  <si>
+    <t>Url path to get the reports download page on System1 website</t>
+  </si>
+  <si>
+    <t>Url path to get the reports page page on System1 website</t>
+  </si>
+  <si>
+    <t>download</t>
+  </si>
+  <si>
+    <t>System1_DownloadFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\dsembiante\Downloads</t>
+  </si>
+  <si>
+    <t>Folder reports are downloaded into</t>
+  </si>
+  <si>
+    <t>System1_MoveFilePath</t>
+  </si>
+  <si>
+    <t>C:\Users\dsembiante\OneDrive - Deloitte (O365D)\UiPathAcademyArcitect\Reports</t>
+  </si>
+  <si>
+    <t>Folder reports are moved into</t>
+  </si>
+  <si>
+    <t>Report-</t>
+  </si>
+  <si>
+    <t>Part of the file path for downlaoded reports</t>
+  </si>
+  <si>
+    <t>System1_ReportNameFilter</t>
+  </si>
+  <si>
+    <t>System1_ReportsUpload</t>
+  </si>
+  <si>
+    <t>upload</t>
+  </si>
+  <si>
+    <t>Url path to get the reports upload page on System1 website</t>
   </si>
 </sst>
 </file>
@@ -573,7 +627,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -683,12 +737,72 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="14" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A14" t="s">
+        <v>69</v>
+      </c>
+      <c r="B14" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" t="s">
+        <v>71</v>
+      </c>
+    </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="17" ht="14.25" customHeight="1"/>

</xml_diff>